<commit_message>
fix: Revise ppt visuals to comply with project specs
</commit_message>
<xml_diff>
--- a/csv-files/popular-family-categories.xlsx
+++ b/csv-files/popular-family-categories.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="categories-barchart1" sheetId="2" r:id="rId1"/>
@@ -594,7 +594,31 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3200"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-ZA" sz="3200"/>
+              <a:t>Family-Friendly</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-ZA" sz="3200" baseline="0"/>
+              <a:t> Categories Total Rentals</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-ZA" sz="3200"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -679,11 +703,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:axId val="101124736"/>
-        <c:axId val="101126528"/>
+        <c:axId val="40796160"/>
+        <c:axId val="40798080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101124736"/>
+        <c:axId val="40796160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -712,7 +736,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101126528"/>
+        <c:crossAx val="40798080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -720,7 +744,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101126528"/>
+        <c:axId val="40798080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,7 +773,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101124736"/>
+        <c:crossAx val="40796160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -765,7 +789,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -776,7 +800,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9299408" cy="6078454"/>
+    <xdr:ext cx="9301574" cy="6079537"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -1088,7 +1112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>